<commit_message>
Update OSMPI Part Management-MPS.xlsx
</commit_message>
<xml_diff>
--- a/General Documentation/OSMPI Part Management-MPS.xlsx
+++ b/General Documentation/OSMPI Part Management-MPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RFLab\Documents\GitHub\MPS\General Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5CE3F4-46A3-4062-B062-78437844E9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55020635-6ADF-49B9-9AF2-8312881A4B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="375">
   <si>
     <t>Magnetic Particle Spectroscopy Project Management Spreadsheet</t>
   </si>
@@ -1140,6 +1140,33 @@
   </si>
   <si>
     <t>For bypass of power supply</t>
+  </si>
+  <si>
+    <t>Misc items:</t>
+  </si>
+  <si>
+    <t>Solder (lead free)</t>
+  </si>
+  <si>
+    <t>Digikey: SMDSWLF.015.3OZ-ND</t>
+  </si>
+  <si>
+    <t>Lead Free No-Clean, Water Soluble Wire Solder Sn96.5Ag3Cu0.5 (96.5/3/0.5) 27 AWG, 28 SWG Tube, 0.3 oz (8.51g)</t>
+  </si>
+  <si>
+    <t>Tweezers</t>
+  </si>
+  <si>
+    <t>Digkey/243-18851-ND</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Digikey/KE1804-ND</t>
+  </si>
+  <si>
+    <t>FLUX PEN FORMULA 951 NO CLEAN</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1677,6 +1704,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5923,15 +5951,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26679483-298F-467F-B7FE-634856DB3200}">
-  <dimension ref="A4:AF23"/>
+  <dimension ref="A4:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
     <col min="3" max="3" width="17.25" customWidth="1"/>
     <col min="4" max="4" width="9.875" customWidth="1"/>
     <col min="5" max="5" width="36.625" bestFit="1" customWidth="1"/>
@@ -6917,6 +6946,41 @@
       <c r="AE23" s="89"/>
       <c r="AF23" s="89"/>
     </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A27" s="105" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A28" s="105" t="s">
+        <v>367</v>
+      </c>
+      <c r="B28" s="105" t="s">
+        <v>368</v>
+      </c>
+      <c r="C28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A29" s="105" t="s">
+        <v>370</v>
+      </c>
+      <c r="B29" s="105" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A30" s="105" t="s">
+        <v>372</v>
+      </c>
+      <c r="B30" s="105" t="s">
+        <v>373</v>
+      </c>
+      <c r="C30" t="s">
+        <v>374</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{8F3FC205-D16F-49E1-AE81-81677CD15645}"/>

</xml_diff>